<commit_message>
Added pca stress results for hatespeech
</commit_message>
<xml_diff>
--- a/Experiments/dimensionality_reduction_metrics/results/other_dr_techniques/PCA/stress_results_PCA.xlsx
+++ b/Experiments/dimensionality_reduction_metrics/results/other_dr_techniques/PCA/stress_results_PCA.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1058,6 +1058,98 @@
         <v>0.170001274791034</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2023-10-02 16:23:58</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>hatespeech</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>10</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.3550838294873909</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2023-10-02 16:24:05</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>hatespeech</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.2604653727803925</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2023-10-02 16:24:05</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>hatespeech</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>30</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.2036138335506539</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2023-10-02 16:24:05</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>hatespeech</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>40</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.1612300686123467</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>